<commit_message>
Multiplayer Game Market Analysis - reference list
</commit_message>
<xml_diff>
--- a/ProjectDocumentation/Appendices/Appendix L - Multiplayer Game Market Analysis/Multiplayer Games Price Analysis.xlsx
+++ b/ProjectDocumentation/Appendices/Appendix L - Multiplayer Game Market Analysis/Multiplayer Games Price Analysis.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentssolihullac-my.sharepoint.com/personal/zek21003166_students_solihull_ac_uk/Documents/Yr3 Final Group Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\ConstructionChaos\ProjectDocumentation\Appendices\Appendix L - Multiplayer Game Market Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{68B87472-D453-4F6A-AA24-1375D94C0603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{435D307C-8974-4997-A5DC-BCF42BDE94E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384A5E6D-C209-49A6-B3B8-61B6A8BD0794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{667E1704-9923-4700-ABF5-15779F4A7210}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="References" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -553,7 +554,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>Super Mario Party</t>
   </si>
@@ -715,6 +716,246 @@
   </si>
   <si>
     <t>Price Range Overall</t>
+  </si>
+  <si>
+    <t>Reference list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Apple (2020). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>App Store</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Apple (United Kingdom). Available at: https://www.apple.com/uk/app-store/ [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Epic Games (2023). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Epic Games Store - Rocket League</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Epicgames.com. Available at: https://store.epicgames.com/en-US/p/rocket-league [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Google (2021). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Android Apps on Google Play</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Google.com. Available at: https://play.google.com/store/games [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft (2023). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Microsoft Apps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Microsoft.com. Available at: https://apps.microsoft.com/store/apps [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nintendo (2023). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Home | My Nintendo Store</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Nintendo UK. Available at: https://store.nintendo.co.uk/en?gclid=Cj0KCQjw7PCjBhDwARIsANo7CgndeDlAphNmafbGRCuTVdrqnEiEc08_3BRAhwmnUSfBgyAwhGNZit8aAn4XEALw_wcB&amp;gad=1&amp;gclsrc=aw.ds [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Playstation (2023). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Latest | Official PlayStation</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>TM</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Store UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Playstation.com. Available at: https://store.playstation.com/en-gb/pages/latest [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steam (2022). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Steam Store</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Steampowered.com. Available at: https://store.steampowered.com/ [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wald, H., Mercante, A., Gerblick, J. and Donnelly, J. (2022). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The 25 best party games to play at home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] gamesradar. Available at: https://www.gamesradar.com/best-party-games/ [Accessed 4 Jun. 2023].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Xbox (2023). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Xbox Official Site: Consoles, Games and Community | Xbox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. [online] Xbox.com. Available at: https://www.xbox.com/en-gb/ [Accessed 4 Jun. 2023].</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -725,7 +966,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +1014,33 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -842,10 +1110,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,19 +1117,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1231,32 +1503,32 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
     </row>
@@ -1282,9 +1554,9 @@
       <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1303,8 +1575,8 @@
       <c r="Q2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
       <c r="T2" s="3" t="s">
         <v>38</v>
       </c>
@@ -1314,7 +1586,7 @@
       <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="17"/>
+      <c r="W2" s="10"/>
       <c r="X2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1331,15 +1603,15 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="13"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9">
+      <c r="I3" s="11"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7">
         <v>49.99</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="T3" s="5">
         <f>MIN(L3:Q3)</f>
         <v>49.99</v>
@@ -1378,23 +1650,23 @@
       <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="L4" s="9">
+      <c r="I4" s="11"/>
+      <c r="L4" s="7">
         <v>24.99</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="7">
         <v>24.99</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <v>24.99</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>25.99</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="7">
         <v>24.09</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="7">
         <v>24.09</v>
       </c>
       <c r="T4" s="5">
@@ -1427,19 +1699,19 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="13"/>
-      <c r="L5" s="9">
+      <c r="I5" s="11"/>
+      <c r="L5" s="7">
         <v>12.99</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7">
         <v>12.99</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>17.989999999999998</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
       <c r="T5" s="5">
         <f t="shared" si="0"/>
         <v>12.99</v>
@@ -1472,21 +1744,21 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="13"/>
-      <c r="L6" s="9">
+      <c r="I6" s="11"/>
+      <c r="L6" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
       <c r="T6" s="5">
         <f t="shared" si="0"/>
         <v>19.989999999999998</v>
@@ -1515,15 +1787,15 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="13"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9">
+      <c r="I7" s="11"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7">
         <v>15.99</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="T7" s="5">
         <f t="shared" si="0"/>
         <v>15.99</v>
@@ -1552,15 +1824,15 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="13"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9">
+      <c r="I8" s="11"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7">
         <v>49.99</v>
       </c>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
       <c r="T8" s="5">
         <f t="shared" si="0"/>
         <v>49.99</v>
@@ -1589,15 +1861,15 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="13"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9">
+      <c r="I9" s="11"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7">
         <v>15.99</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
       <c r="T9" s="5">
         <f t="shared" si="0"/>
         <v>15.99</v>
@@ -1630,19 +1902,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="13"/>
-      <c r="L10" s="9">
+      <c r="I10" s="11"/>
+      <c r="L10" s="7">
         <v>14.99</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="7">
         <v>15.99</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="7">
         <v>15.99</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
       <c r="T10" s="5">
         <f t="shared" si="0"/>
         <v>14.99</v>
@@ -1677,21 +1949,21 @@
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="13"/>
-      <c r="L11" s="9">
+      <c r="I11" s="11"/>
+      <c r="L11" s="7">
         <v>8.5</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="7">
         <v>7.99</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="7">
         <v>8.99</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
       <c r="T11" s="5">
         <f t="shared" si="0"/>
         <v>7.99</v>
@@ -1726,21 +1998,21 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="13"/>
-      <c r="L12" s="9">
+      <c r="I12" s="11"/>
+      <c r="L12" s="7">
         <v>0</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="7">
         <v>0</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <v>0</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="7">
         <v>0</v>
       </c>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
       <c r="T12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1775,21 +2047,21 @@
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="13"/>
-      <c r="L13" s="9">
+      <c r="I13" s="11"/>
+      <c r="L13" s="7">
         <v>12.79</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="7">
         <v>11.99</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="7">
         <v>11.99</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="7">
         <v>13.49</v>
       </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
       <c r="T13" s="5">
         <f t="shared" si="0"/>
         <v>11.99</v>
@@ -1818,15 +2090,15 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="13"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9">
+      <c r="I14" s="11"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7">
         <v>59.99</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
       <c r="T14" s="5">
         <f t="shared" si="0"/>
         <v>59.99</v>
@@ -1859,19 +2131,19 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="13"/>
-      <c r="L15" s="9">
+      <c r="I15" s="11"/>
+      <c r="L15" s="7">
         <v>8.5</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="7">
         <v>7.99</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <v>8.99</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
       <c r="T15" s="5">
         <f t="shared" si="0"/>
         <v>7.99</v>
@@ -1906,21 +2178,21 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="13"/>
-      <c r="L16" s="9">
+      <c r="I16" s="11"/>
+      <c r="L16" s="7">
         <v>10.99</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <v>11.99</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="7">
         <v>11.99</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="7">
         <v>11.79</v>
       </c>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
       <c r="T16" s="5">
         <f t="shared" si="0"/>
         <v>10.99</v>
@@ -1953,19 +2225,19 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="13"/>
-      <c r="L17" s="9">
+      <c r="I17" s="11"/>
+      <c r="L17" s="7">
         <v>8.5</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="M17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
       <c r="T17" s="5">
         <f t="shared" si="0"/>
         <v>8.5</v>
@@ -1998,19 +2270,19 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="13"/>
-      <c r="L18" s="9">
+      <c r="I18" s="11"/>
+      <c r="L18" s="7">
         <v>15.99</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="7">
         <v>15.99</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <v>15.99</v>
       </c>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
       <c r="T18" s="5">
         <f t="shared" si="0"/>
         <v>15.99</v>
@@ -2045,21 +2317,21 @@
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="13"/>
-      <c r="L19" s="9">
+      <c r="I19" s="11"/>
+      <c r="L19" s="7">
         <v>10.99</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="7">
         <v>11.99</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="7">
         <v>14.99</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="7">
         <v>11.99</v>
       </c>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
       <c r="T19" s="5">
         <f t="shared" si="0"/>
         <v>10.99</v>
@@ -2094,21 +2366,21 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="13"/>
-      <c r="L20" s="9">
+      <c r="I20" s="11"/>
+      <c r="L20" s="7">
         <v>10.99</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="7">
         <v>11.99</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="7">
         <v>11.49</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="O20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
       <c r="T20" s="5">
         <f t="shared" si="0"/>
         <v>10.99</v>
@@ -2143,21 +2415,21 @@
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="13"/>
-      <c r="L21" s="9">
+      <c r="I21" s="11"/>
+      <c r="L21" s="7">
         <v>9.99</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="7">
         <v>11.99</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="7">
         <v>13.99</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="7">
         <v>15.29</v>
       </c>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
       <c r="T21" s="5">
         <f t="shared" si="0"/>
         <v>9.99</v>
@@ -2190,19 +2462,19 @@
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="13"/>
-      <c r="L22" s="9">
+      <c r="I22" s="11"/>
+      <c r="L22" s="7">
         <v>10.99</v>
       </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7">
         <v>11.59</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="O22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
       <c r="T22" s="5">
         <f t="shared" si="0"/>
         <v>10.99</v>
@@ -2237,21 +2509,21 @@
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="13"/>
-      <c r="L23" s="9">
+      <c r="I23" s="11"/>
+      <c r="L23" s="7">
         <v>12.79</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="7">
         <v>12.49</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23" s="7">
         <v>11.99</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23" s="7">
         <v>13.49</v>
       </c>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
       <c r="T23" s="5">
         <f t="shared" si="0"/>
         <v>11.99</v>
@@ -2280,15 +2552,15 @@
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="13"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9">
+      <c r="I24" s="11"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7">
         <v>49.99</v>
       </c>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
       <c r="T24" s="5">
         <f t="shared" si="0"/>
         <v>49.99</v>
@@ -2319,17 +2591,17 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="13"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9">
+      <c r="I25" s="11"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7">
         <v>33.49</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N25" s="7">
         <v>32.99</v>
       </c>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
       <c r="T25" s="5">
         <f t="shared" si="0"/>
         <v>32.99</v>
@@ -2362,19 +2634,19 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="13"/>
-      <c r="L26" s="9">
+      <c r="I26" s="11"/>
+      <c r="L26" s="7">
         <v>0</v>
       </c>
-      <c r="M26" s="9" t="s">
+      <c r="M26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="9" t="s">
+      <c r="N26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
       <c r="T26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2409,21 +2681,21 @@
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="13"/>
-      <c r="L27" s="9">
+      <c r="I27" s="11"/>
+      <c r="L27" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="7">
         <v>19.989999999999998</v>
       </c>
-      <c r="O27" s="9" t="s">
+      <c r="O27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
       <c r="T27" s="5">
         <f t="shared" si="0"/>
         <v>19.989999999999998</v>
@@ -2462,23 +2734,23 @@
       <c r="H28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="L28" s="9">
+      <c r="I28" s="11"/>
+      <c r="L28" s="7">
         <v>3.99</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="7">
         <v>4.1900000000000004</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="7">
         <v>3.29</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28" s="7">
         <v>2.72</v>
       </c>
-      <c r="P28" s="9">
+      <c r="P28" s="7">
         <v>0</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="Q28" s="7">
         <v>0</v>
       </c>
       <c r="T28" s="5">
@@ -2507,15 +2779,15 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="13"/>
-      <c r="L29" s="9">
+      <c r="I29" s="11"/>
+      <c r="L29" s="7">
         <v>11.39</v>
       </c>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
       <c r="T29" s="5">
         <f t="shared" ref="T29" si="6">MIN(L29:Q29)</f>
         <v>11.39</v>
@@ -2530,11 +2802,8 @@
       </c>
       <c r="X29" s="4"/>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="I30" s="14"/>
-    </row>
     <row r="31" spans="2:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="3">
@@ -2561,91 +2830,91 @@
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="15" t="s">
+      <c r="I31" s="10"/>
+      <c r="J31" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="8">
         <f>MIN(L3:L29)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="8">
         <f t="shared" ref="M31:Q31" si="10">MIN(M3:M29)</f>
         <v>0</v>
       </c>
-      <c r="N31" s="10">
+      <c r="N31" s="8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O31" s="10">
+      <c r="O31" s="8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P31" s="10">
+      <c r="P31" s="8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="10">
+      <c r="Q31" s="8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="S31" s="15" t="s">
+      <c r="S31" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="12">
         <f t="shared" ref="T31:U31" si="11">MIN(T3:T29)</f>
         <v>0</v>
       </c>
-      <c r="U31" s="16">
+      <c r="U31" s="12">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="15"/>
-      <c r="K32" s="11" t="s">
+      <c r="J32" s="14"/>
+      <c r="K32" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="8">
         <f>MAX(L3:L29)</f>
         <v>24.99</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="8">
         <f t="shared" ref="M32:Q32" si="12">MAX(M3:M29)</f>
         <v>33.49</v>
       </c>
-      <c r="N32" s="10">
+      <c r="N32" s="8">
         <f t="shared" si="12"/>
         <v>32.99</v>
       </c>
-      <c r="O32" s="10">
+      <c r="O32" s="8">
         <f t="shared" si="12"/>
         <v>59.99</v>
       </c>
-      <c r="P32" s="10">
+      <c r="P32" s="8">
         <f t="shared" si="12"/>
         <v>24.09</v>
       </c>
-      <c r="Q32" s="10">
+      <c r="Q32" s="8">
         <f t="shared" si="12"/>
         <v>24.09</v>
       </c>
-      <c r="S32" s="15"/>
-      <c r="T32" s="16">
+      <c r="S32" s="14"/>
+      <c r="T32" s="12">
         <f t="shared" ref="T32:U32" si="13">MAX(T3:T29)</f>
         <v>59.99</v>
       </c>
-      <c r="U32" s="16">
+      <c r="U32" s="12">
         <f t="shared" si="13"/>
         <v>59.99</v>
       </c>
     </row>
     <row r="33" spans="10:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="15"/>
-      <c r="K33" s="11" t="s">
+      <c r="J33" s="14"/>
+      <c r="K33" s="9" t="s">
         <v>49</v>
       </c>
       <c r="L33" s="2" t="str">
@@ -2672,7 +2941,7 @@
         <f t="shared" si="14"/>
         <v>£0 - £24.09</v>
       </c>
-      <c r="S33" s="15"/>
+      <c r="S33" s="14"/>
       <c r="T33" s="2" t="str">
         <f t="shared" si="14"/>
         <v>£0 - £59.99</v>
@@ -2709,4 +2978,97 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1EAD1E-A9BF-4C8E-8722-4D493271336D}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+    </row>
+    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>